<commit_message>
Terminado el archivo de excel
</commit_message>
<xml_diff>
--- a/asistencias.xlsx
+++ b/asistencias.xlsx
@@ -1,41 +1,96 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Documents\proyecto_SS\QR\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A85595-AE8F-4912-8C0D-6763CB4621D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Apellido</t>
+  </si>
+  <si>
+    <t>Número de Alumno</t>
+  </si>
+  <si>
+    <t>2025-03-27</t>
+  </si>
+  <si>
+    <t>Diego</t>
+  </si>
+  <si>
+    <t>Cruz</t>
+  </si>
+  <si>
+    <t>Gael</t>
+  </si>
+  <si>
+    <t>Franco</t>
+  </si>
+  <si>
+    <t>Jonathan</t>
+  </si>
+  <si>
+    <t>Hernandez</t>
+  </si>
+  <si>
+    <t>Juan</t>
+  </si>
+  <si>
+    <t>Martínez</t>
+  </si>
+  <si>
+    <t>✔</t>
+  </si>
+  <si>
+    <t>Rodolfo</t>
+  </si>
+  <si>
+    <t>Alcántara</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0000FF00"/>
-        <bgColor rgb="0000FF00"/>
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FF00FF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -52,81 +107,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -414,120 +410,86 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Nombre</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Apellido</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Número de Alumno</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>2025-03-25</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Diego</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Cruz</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Gael</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Franco</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Jonathan</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Hernandez</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Juan</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Martínez</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Rodolfo</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Alcántara</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
         <v>6</v>
-      </c>
-      <c r="D6" s="1" t="n"/>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>2025-03-25 05:23:27</t>
-        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bastantes cambios, aun falta corregir la interfaz
</commit_message>
<xml_diff>
--- a/asistencias.xlsx
+++ b/asistencias.xlsx
@@ -1,96 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Documents\proyecto_SS\QR\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A85595-AE8F-4912-8C0D-6763CB4621D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>Apellido</t>
-  </si>
-  <si>
-    <t>Número de Alumno</t>
-  </si>
-  <si>
-    <t>2025-03-27</t>
-  </si>
-  <si>
-    <t>Diego</t>
-  </si>
-  <si>
-    <t>Cruz</t>
-  </si>
-  <si>
-    <t>Gael</t>
-  </si>
-  <si>
-    <t>Franco</t>
-  </si>
-  <si>
-    <t>Jonathan</t>
-  </si>
-  <si>
-    <t>Hernandez</t>
-  </si>
-  <si>
-    <t>Juan</t>
-  </si>
-  <si>
-    <t>Martínez</t>
-  </si>
-  <si>
-    <t>✔</t>
-  </si>
-  <si>
-    <t>Rodolfo</t>
-  </si>
-  <si>
-    <t>Alcántara</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00FF00"/>
-        <bgColor rgb="FF00FF00"/>
+        <fgColor rgb="0000FF00"/>
+        <bgColor rgb="0000FF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -107,22 +53,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -410,87 +415,72 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Nombre</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Apellido</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Número de Alumno</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>2025-03-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Diego</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Cruz</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" s="1" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Zaira</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Cruz</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6">
-        <v>6</v>
-      </c>
+      <c r="D3" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Finalizado con las funciones principales
</commit_message>
<xml_diff>
--- a/asistencias.xlsx
+++ b/asistencias.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,11 @@
           <t>2025-03-30</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -465,6 +470,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="n"/>
+      <c r="E2" s="1" t="n"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -481,6 +487,56 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="n"/>
+      <c r="E3" s="1" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Aaron</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Javier</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="n"/>
+      <c r="E4" s="1" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Gael</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Franco</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>uno</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Finalizado el proyecto Version 1.0
</commit_message>
<xml_diff>
--- a/asistencias.xlsx
+++ b/asistencias.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,41 +446,50 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-04-23</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>2025-04-24</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Diego</t>
+          <t>Armando</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Cruz</t>
+          <t>Díaz</t>
         </is>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="n"/>
-      <c r="E2" s="1" t="n"/>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Zaira</t>
+          <t>Cristian</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Cruz</t>
+          <t>Quintero</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -488,16 +497,21 @@
       </c>
       <c r="D3" s="1" t="n"/>
       <c r="E3" s="1" t="n"/>
+      <c r="F3" s="1" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Aaron</t>
+          <t>Javier</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Javier</t>
+          <t>Miranda</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -505,38 +519,432 @@
       </c>
       <c r="D4" s="1" t="n"/>
       <c r="E4" s="1" t="n"/>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Gael</t>
+          <t>Nataly</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Franco</t>
+          <t>García</t>
         </is>
       </c>
       <c r="C5" t="n">
         <v>4</v>
       </c>
-      <c r="D5" s="1" t="n"/>
+      <c r="E5" s="1" t="n"/>
+      <c r="F5" s="1" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Prueba</t>
+          <t>Angelo</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>uno</t>
+          <t>Garcia</t>
         </is>
       </c>
       <c r="C6" t="n">
         <v>5</v>
       </c>
-      <c r="E6" s="1" t="n"/>
+      <c r="F6" s="1" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Yoselin</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Reyes</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>7</v>
+      </c>
+      <c r="F7" s="1" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Jesus</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Martinez</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>6</v>
+      </c>
+      <c r="F8" s="1" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Miguel</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Collin</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>8</v>
+      </c>
+      <c r="F9" s="1" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Edgar</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Miranda</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>9</v>
+      </c>
+      <c r="F10" s="1" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Rosas</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Santiago</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>10</v>
+      </c>
+      <c r="F11" s="1" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Cristian</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Gabriel</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>11</v>
+      </c>
+      <c r="F12" s="1" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Adrian</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Martínez</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>12</v>
+      </c>
+      <c r="F13" s="1" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Wendy</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Santiago</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>13</v>
+      </c>
+      <c r="F14" s="1" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Alexis</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Miranda</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>14</v>
+      </c>
+      <c r="F15" s="1" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Javier</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Cruz</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>15</v>
+      </c>
+      <c r="F16" s="1" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Zuriel</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Fernando</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>16</v>
+      </c>
+      <c r="F17" s="1" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Leo</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Manuel</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>18</v>
+      </c>
+      <c r="F18" s="1" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Emmanuel</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Medina</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>17</v>
+      </c>
+      <c r="F19" s="1" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Uriel</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Camacho</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>20</v>
+      </c>
+      <c r="F20" s="1" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Emanuel</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Cresensiano</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>19</v>
+      </c>
+      <c r="F21" s="1" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Adair</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Antonio</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>21</v>
+      </c>
+      <c r="F22" s="1" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Alexis</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Hernández</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>22</v>
+      </c>
+      <c r="F23" s="1" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Emilio</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Galvan</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>24</v>
+      </c>
+      <c r="F24" s="1" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Josue</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Gregorio</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>23</v>
+      </c>
+      <c r="F25" s="1" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>